<commit_message>
Cleaning code; added enunciados
</commit_message>
<xml_diff>
--- a/files/timesheet_2.xlsx
+++ b/files/timesheet_2.xlsx
@@ -723,8 +723,8 @@
   </sheetPr>
   <dimension ref="A2:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,15 +815,15 @@
       </c>
       <c r="E9" s="34"/>
       <c r="F9" s="34">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G9" s="38">
         <f>SUM(D9:D11)*60+SUM(F9:F11)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H9" s="35" t="str">
         <f>CONCATENATE(QUOTIENT(G9,60),"h",IF(MOD(G9,60)&lt;10,"0",""),MOD(G9,60),"m")</f>
-        <v>0h00m</v>
+        <v>1h30m</v>
       </c>
       <c r="K9" s="1"/>
     </row>
@@ -838,7 +838,7 @@
       </c>
       <c r="E10" s="34"/>
       <c r="F10" s="34">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G10" s="38"/>
       <c r="H10" s="36"/>
@@ -854,7 +854,7 @@
       </c>
       <c r="E11" s="34"/>
       <c r="F11" s="34">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G11" s="38"/>
       <c r="H11" s="36"/>
@@ -868,7 +868,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="34">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E12" s="34"/>
       <c r="F12" s="34">
@@ -876,11 +876,11 @@
       </c>
       <c r="G12" s="38">
         <f>SUM(D12:D13)*60+SUM(F12:F13)</f>
-        <v>0</v>
+        <v>930</v>
       </c>
       <c r="H12" s="35" t="str">
         <f>CONCATENATE(QUOTIENT(G12,60),"h",IF(MOD(G12,60)&lt;10,"0",""),MOD(G12,60),"m")</f>
-        <v>0h00m</v>
+        <v>15h30m</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -894,7 +894,7 @@
       </c>
       <c r="E13" s="34"/>
       <c r="F13" s="34">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G13" s="38"/>
       <c r="H13" s="36"/>
@@ -915,15 +915,15 @@
       </c>
       <c r="E14" s="34"/>
       <c r="F14" s="34">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G14" s="38">
         <f>SUM(D14:D16)*60+SUM(F14:F16)</f>
-        <v>0</v>
+        <v>1595</v>
       </c>
       <c r="H14" s="35" t="str">
         <f>CONCATENATE(QUOTIENT(G14,60),"h",IF(MOD(G14,60)&lt;10,"0",""),MOD(G14,60),"m")</f>
-        <v>0h00m</v>
+        <v>26h35m</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -933,7 +933,7 @@
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="34">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E15" s="34"/>
       <c r="F15" s="34">
@@ -953,7 +953,7 @@
       </c>
       <c r="E16" s="34"/>
       <c r="F16" s="34">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G16" s="38"/>
       <c r="H16" s="36"/>
@@ -976,11 +976,11 @@
       </c>
       <c r="G18" s="17">
         <f>SUM(G9:G16)</f>
-        <v>0</v>
+        <v>2615</v>
       </c>
       <c r="H18" s="23" t="str">
         <f>CONCATENATE(QUOTIENT(G18,60),"h",IF(MOD(G18,60)&lt;10,"0",""),MOD(G18,60),"m")</f>
-        <v>0h00m</v>
+        <v>43h35m</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>